<commit_message>
added new sample map
</commit_message>
<xml_diff>
--- a/maps.xlsx
+++ b/maps.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\slam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AD5137-FC32-4D4D-ACC5-ADC6E24D399A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33CAC73-34D3-4D7A-B14F-3512142210C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet0" sheetId="16" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="10" r:id="rId9"/>
-    <sheet name="Sheet9" sheetId="11" r:id="rId10"/>
-    <sheet name="Sheet10" sheetId="12" r:id="rId11"/>
-    <sheet name="Sheet11" sheetId="13" r:id="rId12"/>
-    <sheet name="Sheet12" sheetId="14" r:id="rId13"/>
-    <sheet name="DEMO" sheetId="15" r:id="rId14"/>
+    <sheet name="Sheet00" sheetId="16" r:id="rId1"/>
+    <sheet name="Sheet01" sheetId="17" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet7" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet9" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet10" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet11" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet12" sheetId="14" r:id="rId14"/>
+    <sheet name="DEMO" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="40">
   <si>
     <t>col1</t>
   </si>
@@ -586,15 +587,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444943E8-FCD1-46B6-9C60-770E2EC278E9}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -610,31 +609,43 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>-255</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
@@ -644,10 +655,16 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -661,10 +678,16 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -673,27 +696,85 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>255</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -703,6 +784,442 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37AE3D1-6097-4711-BC60-EEDCC75CB075}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3">
+        <v>255</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>-255</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51333FAB-9D50-443F-9322-F9DDD983843B}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -1138,7 +1655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53924B42-3909-4272-A548-B312509CF1B3}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
@@ -2755,7 +3272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EDB805-B65E-44FA-9E03-634BCBD8A426}">
   <dimension ref="A1:V23"/>
   <sheetViews>
@@ -4335,7 +4852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBDFE4C-82FE-449D-BDDB-F4DDC63E2E22}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -4720,7 +5237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025B5C29-5A33-4366-8D13-666287F14682}">
   <dimension ref="A1:N29"/>
   <sheetViews>
@@ -5588,6 +6105,206 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB10D7C-E3EC-43C0-A97F-BC0787C4E680}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="A1:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>-255</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>255</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W23"/>
   <sheetViews>
@@ -7239,7 +7956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD033E48-BD4B-4984-B655-F119C77DB1ED}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -7541,7 +8258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCB3AC8-2E2B-4FCD-BC88-ABFD876CE37E}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -7846,7 +8563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A97B2D0-D2DB-456A-B7F3-9AB54BCD355F}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -8048,7 +8765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52962A5-C9BA-4DED-944D-D973B99E56D9}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -8227,7 +8944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA649F3C-9117-4912-8352-7DDFBD834BCF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -8385,7 +9102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E91400-1737-4A4C-B7EB-871828932665}">
   <dimension ref="A1:M11"/>
   <sheetViews>
@@ -8848,440 +9565,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37AE3D1-6097-4711-BC60-EEDCC75CB075}">
-  <dimension ref="A1:L11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3">
-        <v>255</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>-255</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>